<commit_message>
spreadsheets: On Delivery Locations, make country a drop down menu
Also make sure all tabs start in top left corner
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_v007.xlsx
+++ b/indigo/spreadsheetform_guides/project_v007.xlsx
@@ -28,6 +28,7 @@
     <sheet name="Results" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Open Contracting" sheetId="19" state="visible" r:id="rId20"/>
     <sheet name="360Giving" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="CountryCodeOptions" sheetId="21" state="hidden" r:id="rId22"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="803">
   <si>
     <t xml:space="preserve">INDIGO Project ID</t>
   </si>
@@ -1750,6 +1751,750 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:360giving_datas:status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZW</t>
   </si>
 </sst>
 </file>
@@ -2436,7 +3181,7 @@
   </sheetPr>
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3210,7 +3955,7 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3696,7 +4441,7 @@
   <dimension ref="A2:R33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S34" activeCellId="0" sqref="S34"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4483,7 +5228,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6166,8 +6911,8 @@
   </sheetPr>
   <dimension ref="A1:A57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8305,7 +9050,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8527,6 +9272,1278 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A249"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A249" activeCellId="0" sqref="A249"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>802</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -9061,7 +11078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
         <v>204</v>
       </c>
@@ -9498,9 +11515,13 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L4:L32" type="list">
       <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4:D32" type="list">
+      <formula1>CountryCodeOptions!$A$1:$A$249</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -9941,7 +11962,7 @@
   <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10426,7 +12447,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11007,7 +13028,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11701,7 +13722,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>